<commit_message>
changed new google form
</commit_message>
<xml_diff>
--- a/TodayFolders/SecondProjectSpreadsheet.xlsx
+++ b/TodayFolders/SecondProjectSpreadsheet.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ebcbcc0fd1acfae9/ドキュメント/Excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC10484AD118556A5ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4D3EEB3-1571-41CA-A198-39D63B91E6E3}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_F25DC773A252ABDACC10484AD118556A5ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44DB5228-0DC6-4BE0-98DF-21E9642F143C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Spreadsheet" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,101 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
   <si>
-    <t>Horodateur</t>
+    <t>Timestamp</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Please select name </t>
+    <t>霊園名</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Enter billing amount Ex) 100,000¥</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20/05/2022 02:01:12</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Seishoin</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>55￥</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20/05/2022 02:01:45</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>shumatokaido</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>500¥</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20/05/2022 02:02:27</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Honchoji Temple</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>100¥</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Horodateur</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Please select name </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Enter billing amount Ex) 100,000¥</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20/05/2022 02:01:12</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Seishoin</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>55￥</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20/05/2022 02:01:45</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>shumatokaido</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>500¥</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20/05/2022 02:02:27</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Honchoji Temple</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>100¥</t>
+    <t>ご請求額を入力して下さい。例 ¥100,000</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -128,7 +43,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,16 +53,6 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -174,11 +79,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,127 +360,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F473A9-F585-4FB9-9F31-D6DE6C09DF3F}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="26.875" customWidth="1"/>
-    <col min="3" max="3" width="33.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC40711-55DB-423B-AB9E-444BEE93EB0E}">
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>